<commit_message>
added facebook post structure
</commit_message>
<xml_diff>
--- a/FB Page Links All.xlsx
+++ b/FB Page Links All.xlsx
@@ -5,17 +5,20 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rh\Dropbox\Research\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacob\Documents\Projects\FacebookCompanyScraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985"/>
   </bookViews>
   <sheets>
     <sheet name="FB Links" sheetId="1" r:id="rId1"/>
     <sheet name="InfoNeeded" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="hidden" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7852" uniqueCount="4660">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7852" uniqueCount="4662">
   <si>
     <t>1-800 FLOWERS COM FLWS</t>
   </si>
@@ -14006,6 +14009,12 @@
   </si>
   <si>
     <t>FB link</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/providentfinancial</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/VPGinc</t>
   </si>
 </sst>
 </file>
@@ -14062,8 +14071,36 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -14340,8 +14377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1596"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A1156" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1181" sqref="C1181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27338,7 +27375,7 @@
         <v>3383</v>
       </c>
       <c r="C1181" t="s">
-        <v>3384</v>
+        <v>4660</v>
       </c>
     </row>
     <row r="1182" spans="1:3" x14ac:dyDescent="0.25">
@@ -31056,7 +31093,7 @@
         <v>4389</v>
       </c>
       <c r="C1519" t="s">
-        <v>4390</v>
+        <v>4661</v>
       </c>
     </row>
     <row r="1520" spans="1:3" x14ac:dyDescent="0.25">
@@ -31909,6 +31946,7 @@
   </sheetData>
   <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>